<commit_message>
Update emissions factors for SOx and PMS for diesel, biodiesel and methanol ships
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-final-energy.xlsx
+++ b/premise/data/additional_inventories/lci-final-energy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA164E1-D8BB-234F-A65E-B31857B616D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{894C046D-FCF4-3340-8C72-6433DB7B3A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2620" yWindow="760" windowWidth="25800" windowHeight="18880" xr2:uid="{B8299F2D-33B8-E148-B485-6429887DEB23}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9143" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9137" uniqueCount="405">
   <si>
     <t>database</t>
   </si>
@@ -1254,25 +1254,35 @@
   <si>
     <t>heat, residential, by combustion of methanol using boiler, distributed by truck, produced by Electrolysis, PEM using electricity from grid and carbon sourced from DAC</t>
   </si>
+  <si>
+    <t>SOx emissions have been updated to reflect the use of VLSFO.</t>
+  </si>
+  <si>
+    <t>Wartsila reports an emission factor of about 0.7g NOx/MJ methanol: https://www.wartsila.com/insights/article/next-port-of-call-the-methanol-bunkering-station
+In teh same report, they also report a reduction of 90% of PM emissions compared to using HFO.</t>
+  </si>
+  <si>
+    <t>We assume the absence of sulfur in synthetic diesel. Additionally, according to Petzold et al., 2011, dx.doi.org/10.1021/es2021439, there's a reduction of about 60% in PM emissions relative to using HFO.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="13">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="0.000000"/>
-    <numFmt numFmtId="167" formatCode="0.0E+00"/>
-    <numFmt numFmtId="168" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="169" formatCode="0.00000"/>
-    <numFmt numFmtId="170" formatCode="0.0000000"/>
-    <numFmt numFmtId="171" formatCode="_ * #,##0.00000_ ;_ * \-#,##0.00000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="172" formatCode="_ * #,##0.000000_ ;_ * \-#,##0.000000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="173" formatCode="0.000"/>
-    <numFmt numFmtId="174" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="175" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;-&quot;?_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.000000"/>
+    <numFmt numFmtId="168" formatCode="0.0E+00"/>
+    <numFmt numFmtId="169" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="170" formatCode="0.00000"/>
+    <numFmt numFmtId="171" formatCode="0.0000000"/>
+    <numFmt numFmtId="172" formatCode="_ * #,##0.00000_ ;_ * \-#,##0.00000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="173" formatCode="_ * #,##0.000000_ ;_ * \-#,##0.000000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="174" formatCode="0.000"/>
+    <numFmt numFmtId="175" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;-&quot;?_ ;_ @_ "/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -1350,24 +1360,24 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1381,28 +1391,32 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1721,8 +1735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F0C42E2-D17A-554B-A2D9-4F73B84316EE}">
   <dimension ref="A1:O3102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1284" zoomScale="125" workbookViewId="0">
-      <selection activeCell="K1302" sqref="K1302"/>
+    <sheetView tabSelected="1" topLeftCell="A2078" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D2094" sqref="D2094"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -41796,10 +41810,10 @@
     </row>
     <row r="2092" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2092" s="2" t="s">
-        <v>6</v>
+        <v>151</v>
       </c>
       <c r="B2092" s="2" t="s">
-        <v>7</v>
+        <v>402</v>
       </c>
       <c r="C2092" s="2"/>
       <c r="D2092" s="2"/>
@@ -41809,15 +41823,13 @@
       <c r="H2092" s="2"/>
       <c r="I2092" s="2"/>
       <c r="J2092" s="2"/>
-      <c r="K2092" s="2"/>
-      <c r="L2092" s="2"/>
     </row>
     <row r="2093" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2093" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2093" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C2093" s="2"/>
       <c r="D2093" s="2"/>
@@ -41831,10 +41843,12 @@
       <c r="L2093" s="2"/>
     </row>
     <row r="2094" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2094" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2094" s="2"/>
+      <c r="A2094" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2094" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="C2094" s="2"/>
       <c r="D2094" s="2"/>
       <c r="E2094" s="2"/>
@@ -41846,108 +41860,106 @@
       <c r="K2094" s="2"/>
       <c r="L2094" s="2"/>
     </row>
-    <row r="2095" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2095" s="17" t="s">
+    <row r="2095" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2095" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2095" s="2"/>
+      <c r="C2095" s="2"/>
+      <c r="D2095" s="2"/>
+      <c r="E2095" s="2"/>
+      <c r="F2095" s="2"/>
+      <c r="G2095" s="2"/>
+      <c r="H2095" s="2"/>
+      <c r="I2095" s="2"/>
+      <c r="J2095" s="2"/>
+      <c r="K2095" s="2"/>
+      <c r="L2095" s="2"/>
+    </row>
+    <row r="2096" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2096" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B2095" s="17" t="s">
+      <c r="B2096" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C2095" s="17" t="s">
+      <c r="C2096" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D2095" s="17" t="s">
+      <c r="D2096" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E2095" s="17" t="s">
+      <c r="E2096" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F2095" s="17" t="s">
+      <c r="F2096" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G2095" s="17" t="s">
+      <c r="G2096" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I2095" s="17"/>
-      <c r="J2095" s="17"/>
-      <c r="K2095" s="17"/>
-    </row>
-    <row r="2096" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2096" s="2" t="str">
+      <c r="I2096" s="17"/>
+      <c r="J2096" s="17"/>
+      <c r="K2096" s="17"/>
+    </row>
+    <row r="2097" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2097" s="2" t="str">
         <f>B2088</f>
         <v>heavy fuel oil, burned in container ship</v>
       </c>
-      <c r="B2096" s="2">
+      <c r="B2097" s="2">
         <v>1</v>
       </c>
-      <c r="C2096" s="2" t="str">
+      <c r="C2097" s="2" t="str">
         <f>B2089</f>
         <v>RER</v>
       </c>
-      <c r="D2096" s="2"/>
-      <c r="E2096" s="2" t="str">
-        <f>B2093</f>
+      <c r="D2097" s="2"/>
+      <c r="E2097" s="2" t="str">
+        <f>B2094</f>
         <v>megajoule</v>
       </c>
-      <c r="F2096" s="2" t="s">
+      <c r="F2097" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G2096" s="2" t="str">
+      <c r="G2097" s="2" t="str">
         <f>B2091</f>
         <v>heat</v>
       </c>
-      <c r="H2096" s="2"/>
-      <c r="I2096" s="2"/>
-      <c r="J2096" s="2"/>
-      <c r="K2096" s="2"/>
-      <c r="L2096" s="2"/>
-    </row>
-    <row r="2097" spans="1:11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2097" t="s">
+      <c r="H2097" s="2"/>
+      <c r="I2097" s="2"/>
+      <c r="J2097" s="2"/>
+      <c r="K2097" s="2"/>
+      <c r="L2097" s="2"/>
+    </row>
+    <row r="2098" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2098" t="s">
         <v>125</v>
       </c>
-      <c r="B2097">
+      <c r="B2098">
         <f>1/39</f>
         <v>2.564102564102564E-2</v>
       </c>
-      <c r="C2097" t="s">
+      <c r="C2098" t="s">
         <v>27</v>
       </c>
-      <c r="E2097" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2097" t="s">
+      <c r="E2098" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2098" t="s">
         <v>23</v>
       </c>
-      <c r="G2097" t="s">
+      <c r="G2098" t="s">
         <v>102</v>
       </c>
-      <c r="H2097" s="2"/>
-    </row>
-    <row r="2098" spans="1:11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2098" t="s">
+      <c r="H2098" s="2"/>
+    </row>
+    <row r="2099" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2099" t="s">
         <v>48</v>
       </c>
-      <c r="B2098" s="3">
+      <c r="B2099" s="3">
         <v>1.0256365433645409E-5</v>
-      </c>
-      <c r="D2098" t="s">
-        <v>100</v>
-      </c>
-      <c r="E2098" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2098" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2098" s="2"/>
-    </row>
-    <row r="2099" spans="1:11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2099" t="s">
-        <v>90</v>
-      </c>
-      <c r="B2099" s="3">
-        <v>9.6449727337009339E-9</v>
       </c>
       <c r="D2099" t="s">
         <v>100</v>
@@ -41960,12 +41972,12 @@
       </c>
       <c r="H2099" s="2"/>
     </row>
-    <row r="2100" spans="1:11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="2100" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2100" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="B2100" s="3">
-        <v>6.2721921074364377E-10</v>
+        <v>9.6449727337009339E-9</v>
       </c>
       <c r="D2100" t="s">
         <v>100</v>
@@ -41978,12 +41990,12 @@
       </c>
       <c r="H2100" s="2"/>
     </row>
-    <row r="2101" spans="1:11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="2101" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2101" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2101">
-        <v>7.9939098901879183E-2</v>
+        <v>52</v>
+      </c>
+      <c r="B2101" s="3">
+        <v>6.2721921074364377E-10</v>
       </c>
       <c r="D2101" t="s">
         <v>100</v>
@@ -41996,12 +42008,12 @@
       </c>
       <c r="H2101" s="2"/>
     </row>
-    <row r="2102" spans="1:11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="2102" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2102" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2102" s="3">
-        <v>6.8728477177939384E-5</v>
+        <v>53</v>
+      </c>
+      <c r="B2102">
+        <v>7.9939098901879183E-2</v>
       </c>
       <c r="D2102" t="s">
         <v>100</v>
@@ -42013,14 +42025,13 @@
         <v>15</v>
       </c>
       <c r="H2102" s="2"/>
-      <c r="K2102" s="3"/>
-    </row>
-    <row r="2103" spans="1:11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2103" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2103" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2103" s="3">
-        <v>4.0039462777159148E-9</v>
+        <v>6.8728477177939384E-5</v>
       </c>
       <c r="D2103" t="s">
         <v>100</v>
@@ -42034,12 +42045,12 @@
       <c r="H2103" s="2"/>
       <c r="K2103" s="3"/>
     </row>
-    <row r="2104" spans="1:11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="2104" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2104" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B2104" s="3">
-        <v>9.6449727337009339E-9</v>
+        <v>4.0039462777159148E-9</v>
       </c>
       <c r="D2104" t="s">
         <v>100</v>
@@ -42053,12 +42064,12 @@
       <c r="H2104" s="2"/>
       <c r="K2104" s="3"/>
     </row>
-    <row r="2105" spans="1:11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="2105" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2105" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2105" s="3">
-        <v>4.0793809536092252E-6</v>
+        <v>9.6449727337009339E-9</v>
       </c>
       <c r="D2105" t="s">
         <v>100</v>
@@ -42072,12 +42083,12 @@
       <c r="H2105" s="2"/>
       <c r="K2105" s="3"/>
     </row>
-    <row r="2106" spans="1:11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="2106" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2106" t="s">
-        <v>103</v>
+        <v>58</v>
       </c>
       <c r="B2106" s="3">
-        <v>2.5641066388993793E-14</v>
+        <v>4.0793809536092252E-6</v>
       </c>
       <c r="D2106" t="s">
         <v>100</v>
@@ -42089,13 +42100,14 @@
         <v>15</v>
       </c>
       <c r="H2106" s="2"/>
-    </row>
-    <row r="2107" spans="1:11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="K2106" s="3"/>
+    </row>
+    <row r="2107" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2107" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2107" s="3">
-        <v>1.4988121356087533E-6</v>
+        <v>2.5641066388993793E-14</v>
       </c>
       <c r="D2107" t="s">
         <v>100</v>
@@ -42108,12 +42120,12 @@
       </c>
       <c r="H2107" s="2"/>
     </row>
-    <row r="2108" spans="1:11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="2108" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2108" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B2108" s="3">
-        <v>1.4988121356087536E-7</v>
+        <v>1.4988121356087533E-6</v>
       </c>
       <c r="D2108" t="s">
         <v>100</v>
@@ -42126,12 +42138,12 @@
       </c>
       <c r="H2108" s="2"/>
     </row>
-    <row r="2109" spans="1:11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="2109" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2109" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="B2109" s="3">
-        <v>4.4181493731679086E-9</v>
+        <v>1.4988121356087536E-7</v>
       </c>
       <c r="D2109" t="s">
         <v>100</v>
@@ -42144,12 +42156,12 @@
       </c>
       <c r="H2109" s="2"/>
     </row>
-    <row r="2110" spans="1:11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="2110" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2110" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2110" s="3">
-        <v>7.2386626011604185E-10</v>
+        <v>4.4181493731679086E-9</v>
       </c>
       <c r="D2110" t="s">
         <v>100</v>
@@ -42162,12 +42174,12 @@
       </c>
       <c r="H2110" s="2"/>
     </row>
-    <row r="2111" spans="1:11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="2111" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2111" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2111" s="3">
-        <v>1.3879471014768287E-6</v>
+        <v>7.2386626011604185E-10</v>
       </c>
       <c r="D2111" t="s">
         <v>100</v>
@@ -42180,12 +42192,12 @@
       </c>
       <c r="H2111" s="2"/>
     </row>
-    <row r="2112" spans="1:11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="2112" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2112" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B2112" s="3">
-        <v>6.9408357025220894E-5</v>
+        <v>1.3879471014768287E-6</v>
       </c>
       <c r="D2112" t="s">
         <v>100</v>
@@ -42200,10 +42212,10 @@
     </row>
     <row r="2113" spans="1:8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2113" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2113" s="3">
-        <v>5.5818502193524422E-7</v>
+        <v>6.9408357025220894E-5</v>
       </c>
       <c r="D2113" t="s">
         <v>100</v>
@@ -42218,10 +42230,10 @@
     </row>
     <row r="2114" spans="1:8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2114" t="s">
-        <v>69</v>
-      </c>
-      <c r="B2114">
-        <v>1.9128828001645137E-3</v>
+        <v>68</v>
+      </c>
+      <c r="B2114" s="3">
+        <v>5.5818502193524422E-7</v>
       </c>
       <c r="D2114" t="s">
         <v>100</v>
@@ -42236,10 +42248,10 @@
     </row>
     <row r="2115" spans="1:8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2115" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2115" s="3">
-        <v>5.12820309080674E-8</v>
+        <v>69</v>
+      </c>
+      <c r="B2115">
+        <v>1.9128828001645137E-3</v>
       </c>
       <c r="D2115" t="s">
         <v>100</v>
@@ -42254,10 +42266,10 @@
     </row>
     <row r="2116" spans="1:8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2116" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2116" s="3">
-        <v>4.4996554963039493E-5</v>
+        <v>5.12820309080674E-8</v>
       </c>
       <c r="D2116" t="s">
         <v>100</v>
@@ -42272,10 +42284,11 @@
     </row>
     <row r="2117" spans="1:8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2117" t="s">
-        <v>106</v>
+        <v>71</v>
       </c>
       <c r="B2117" s="3">
-        <v>6.428083646287935E-5</v>
+        <f>0.00695*B2098</f>
+        <v>1.782051282051282E-4</v>
       </c>
       <c r="D2117" t="s">
         <v>100</v>
@@ -42293,7 +42306,8 @@
         <v>107</v>
       </c>
       <c r="B2118" s="3">
-        <v>5.1424648796319438E-5</v>
+        <f>0.0006*B2098</f>
+        <v>1.5384615384615384E-5</v>
       </c>
       <c r="D2118" t="s">
         <v>100</v>
@@ -42329,7 +42343,8 @@
         <v>77</v>
       </c>
       <c r="B2120">
-        <v>1.1659114234524397E-3</v>
+        <f>2*97.54%*0.5%*B2098</f>
+        <v>2.5010256410256412E-4</v>
       </c>
       <c r="D2120" t="s">
         <v>100</v>
@@ -42533,10 +42548,10 @@
     </row>
     <row r="2133" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2133" s="2" t="s">
-        <v>8</v>
+        <v>151</v>
       </c>
       <c r="B2133" s="2" t="s">
-        <v>17</v>
+        <v>404</v>
       </c>
       <c r="C2133" s="2"/>
       <c r="D2133" s="2"/>
@@ -42550,10 +42565,12 @@
       <c r="L2133" s="2"/>
     </row>
     <row r="2134" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2134" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2134" s="2"/>
+      <c r="A2134" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2134" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="C2134" s="2"/>
       <c r="D2134" s="2"/>
       <c r="E2134" s="2"/>
@@ -42565,108 +42582,106 @@
       <c r="K2134" s="2"/>
       <c r="L2134" s="2"/>
     </row>
-    <row r="2135" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2135" s="17" t="s">
+    <row r="2135" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2135" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2135" s="2"/>
+      <c r="C2135" s="2"/>
+      <c r="D2135" s="2"/>
+      <c r="E2135" s="2"/>
+      <c r="F2135" s="2"/>
+      <c r="G2135" s="2"/>
+      <c r="H2135" s="2"/>
+      <c r="I2135" s="2"/>
+      <c r="J2135" s="2"/>
+      <c r="K2135" s="2"/>
+      <c r="L2135" s="2"/>
+    </row>
+    <row r="2136" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2136" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B2135" s="17" t="s">
+      <c r="B2136" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C2135" s="17" t="s">
+      <c r="C2136" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D2135" s="17" t="s">
+      <c r="D2136" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E2135" s="17" t="s">
+      <c r="E2136" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F2135" s="17" t="s">
+      <c r="F2136" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G2135" s="17" t="s">
+      <c r="G2136" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I2135" s="17"/>
-      <c r="J2135" s="17"/>
-      <c r="K2135" s="17"/>
-    </row>
-    <row r="2136" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2136" s="2" t="str">
+      <c r="I2136" s="17"/>
+      <c r="J2136" s="17"/>
+      <c r="K2136" s="17"/>
+    </row>
+    <row r="2137" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2137" s="2" t="str">
         <f>B2128</f>
         <v>diesel, synthetic, burned in container ship</v>
       </c>
-      <c r="B2136" s="2">
+      <c r="B2137" s="2">
         <v>1</v>
       </c>
-      <c r="C2136" s="2" t="str">
+      <c r="C2137" s="2" t="str">
         <f>B2129</f>
         <v>RER</v>
       </c>
-      <c r="D2136" s="2"/>
-      <c r="E2136" s="2" t="str">
-        <f>B2133</f>
+      <c r="D2137" s="2"/>
+      <c r="E2137" s="2" t="str">
+        <f>B2134</f>
         <v>megajoule</v>
       </c>
-      <c r="F2136" s="2" t="s">
+      <c r="F2137" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G2136" s="2" t="str">
+      <c r="G2137" s="2" t="str">
         <f>B2131</f>
         <v>heat</v>
       </c>
-      <c r="H2136" s="2"/>
-      <c r="I2136" s="2"/>
-      <c r="J2136" s="2"/>
-      <c r="K2136" s="2"/>
-      <c r="L2136" s="2"/>
-    </row>
-    <row r="2137" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2137" t="s">
+      <c r="H2137" s="2"/>
+      <c r="I2137" s="2"/>
+      <c r="J2137" s="2"/>
+      <c r="K2137" s="2"/>
+      <c r="L2137" s="2"/>
+    </row>
+    <row r="2138" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2138" t="s">
         <v>398</v>
       </c>
-      <c r="B2137">
+      <c r="B2138">
         <f>1/39</f>
         <v>2.564102564102564E-2</v>
       </c>
-      <c r="C2137" t="s">
+      <c r="C2138" t="s">
         <v>18</v>
       </c>
-      <c r="E2137" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2137" t="s">
+      <c r="E2138" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2138" t="s">
         <v>23</v>
       </c>
-      <c r="G2137" t="s">
+      <c r="G2138" t="s">
         <v>133</v>
-      </c>
-      <c r="H2137" s="2"/>
-    </row>
-    <row r="2138" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2138" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2138" s="3">
-        <v>1.0256365433645409E-5</v>
-      </c>
-      <c r="D2138" t="s">
-        <v>100</v>
-      </c>
-      <c r="E2138" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2138" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="H2138" s="2"/>
     </row>
     <row r="2139" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2139" t="s">
-        <v>90</v>
+        <v>48</v>
       </c>
       <c r="B2139" s="3">
-        <v>9.6449727337009339E-9</v>
+        <v>1.0256365433645409E-5</v>
       </c>
       <c r="D2139" t="s">
         <v>100</v>
@@ -42681,10 +42696,10 @@
     </row>
     <row r="2140" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2140" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="B2140" s="3">
-        <v>6.2721921074364377E-10</v>
+        <v>9.6449727337009339E-9</v>
       </c>
       <c r="D2140" t="s">
         <v>100</v>
@@ -42699,11 +42714,10 @@
     </row>
     <row r="2141" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2141" t="s">
-        <v>122</v>
-      </c>
-      <c r="B2141">
-        <f>3.15*B2137</f>
-        <v>8.076923076923076E-2</v>
+        <v>52</v>
+      </c>
+      <c r="B2141" s="3">
+        <v>6.2721921074364377E-10</v>
       </c>
       <c r="D2141" t="s">
         <v>100</v>
@@ -42718,10 +42732,11 @@
     </row>
     <row r="2142" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2142" t="s">
-        <v>123</v>
-      </c>
-      <c r="B2142" s="3">
-        <v>6.8728477177939384E-5</v>
+        <v>122</v>
+      </c>
+      <c r="B2142">
+        <f>3.15*B2138</f>
+        <v>8.076923076923076E-2</v>
       </c>
       <c r="D2142" t="s">
         <v>100</v>
@@ -42733,14 +42748,13 @@
         <v>15</v>
       </c>
       <c r="H2142" s="2"/>
-      <c r="K2142" s="3"/>
     </row>
     <row r="2143" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2143" t="s">
-        <v>55</v>
+        <v>123</v>
       </c>
       <c r="B2143" s="3">
-        <v>4.0039462777159148E-9</v>
+        <v>6.8728477177939384E-5</v>
       </c>
       <c r="D2143" t="s">
         <v>100</v>
@@ -42756,10 +42770,10 @@
     </row>
     <row r="2144" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2144" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B2144" s="3">
-        <v>9.6449727337009339E-9</v>
+        <v>4.0039462777159148E-9</v>
       </c>
       <c r="D2144" t="s">
         <v>100</v>
@@ -42775,10 +42789,10 @@
     </row>
     <row r="2145" spans="1:11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2145" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2145" s="3">
-        <v>4.0793809536092252E-6</v>
+        <v>9.6449727337009339E-9</v>
       </c>
       <c r="D2145" t="s">
         <v>100</v>
@@ -42794,10 +42808,10 @@
     </row>
     <row r="2146" spans="1:11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2146" t="s">
-        <v>103</v>
+        <v>58</v>
       </c>
       <c r="B2146" s="3">
-        <v>2.5641066388993793E-14</v>
+        <v>4.0793809536092252E-6</v>
       </c>
       <c r="D2146" t="s">
         <v>100</v>
@@ -42809,13 +42823,14 @@
         <v>15</v>
       </c>
       <c r="H2146" s="2"/>
+      <c r="K2146" s="3"/>
     </row>
     <row r="2147" spans="1:11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2147" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2147" s="3">
-        <v>1.4988121356087533E-6</v>
+        <v>2.5641066388993793E-14</v>
       </c>
       <c r="D2147" t="s">
         <v>100</v>
@@ -42830,10 +42845,10 @@
     </row>
     <row r="2148" spans="1:11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2148" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B2148" s="3">
-        <v>1.4988121356087536E-7</v>
+        <v>1.4988121356087533E-6</v>
       </c>
       <c r="D2148" t="s">
         <v>100</v>
@@ -42848,10 +42863,10 @@
     </row>
     <row r="2149" spans="1:11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2149" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="B2149" s="3">
-        <v>4.4181493731679086E-9</v>
+        <v>1.4988121356087536E-7</v>
       </c>
       <c r="D2149" t="s">
         <v>100</v>
@@ -42866,10 +42881,10 @@
     </row>
     <row r="2150" spans="1:11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2150" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2150" s="3">
-        <v>7.2386626011604185E-10</v>
+        <v>4.4181493731679086E-9</v>
       </c>
       <c r="D2150" t="s">
         <v>100</v>
@@ -42884,10 +42899,10 @@
     </row>
     <row r="2151" spans="1:11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2151" t="s">
-        <v>177</v>
+        <v>64</v>
       </c>
       <c r="B2151" s="3">
-        <v>1.3879471014768287E-6</v>
+        <v>7.2386626011604185E-10</v>
       </c>
       <c r="D2151" t="s">
         <v>100</v>
@@ -42902,10 +42917,10 @@
     </row>
     <row r="2152" spans="1:11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2152" t="s">
-        <v>67</v>
+        <v>177</v>
       </c>
       <c r="B2152" s="3">
-        <v>6.9408357025220894E-5</v>
+        <v>1.3879471014768287E-6</v>
       </c>
       <c r="D2152" t="s">
         <v>100</v>
@@ -42920,10 +42935,10 @@
     </row>
     <row r="2153" spans="1:11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2153" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2153" s="3">
-        <v>5.5818502193524422E-7</v>
+        <v>6.9408357025220894E-5</v>
       </c>
       <c r="D2153" t="s">
         <v>100</v>
@@ -42938,10 +42953,10 @@
     </row>
     <row r="2154" spans="1:11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2154" t="s">
-        <v>69</v>
-      </c>
-      <c r="B2154">
-        <v>1.9128828001645137E-3</v>
+        <v>68</v>
+      </c>
+      <c r="B2154" s="3">
+        <v>5.5818502193524422E-7</v>
       </c>
       <c r="D2154" t="s">
         <v>100</v>
@@ -42956,10 +42971,10 @@
     </row>
     <row r="2155" spans="1:11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2155" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2155" s="3">
-        <v>5.12820309080674E-8</v>
+        <v>69</v>
+      </c>
+      <c r="B2155">
+        <v>1.9128828001645137E-3</v>
       </c>
       <c r="D2155" t="s">
         <v>100</v>
@@ -42974,10 +42989,10 @@
     </row>
     <row r="2156" spans="1:11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2156" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2156" s="3">
-        <v>4.4996554963039493E-5</v>
+        <v>5.12820309080674E-8</v>
       </c>
       <c r="D2156" t="s">
         <v>100</v>
@@ -42992,10 +43007,11 @@
     </row>
     <row r="2157" spans="1:11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2157" t="s">
-        <v>106</v>
+        <v>71</v>
       </c>
       <c r="B2157" s="3">
-        <v>6.428083646287935E-5</v>
+        <f>0.00695*B2138*(1-0.6)</f>
+        <v>7.1282051282051278E-5</v>
       </c>
       <c r="D2157" t="s">
         <v>100</v>
@@ -43013,7 +43029,8 @@
         <v>107</v>
       </c>
       <c r="B2158" s="3">
-        <v>5.1424648796319438E-5</v>
+        <f>0.0006*B2138*(1-0.6)</f>
+        <v>6.153846153846154E-6</v>
       </c>
       <c r="D2158" t="s">
         <v>100</v>
@@ -43046,10 +43063,10 @@
     </row>
     <row r="2160" spans="1:11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2160" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2160">
-        <v>1.1659114234524397E-3</v>
+        <v>79</v>
+      </c>
+      <c r="B2160" s="3">
+        <v>2.0260399075004886E-8</v>
       </c>
       <c r="D2160" t="s">
         <v>100</v>
@@ -43064,13 +43081,13 @@
     </row>
     <row r="2161" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2161" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="B2161" s="3">
-        <v>2.0260399075004886E-8</v>
+        <v>1.6520143085674979E-9</v>
       </c>
       <c r="D2161" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="E2161" t="s">
         <v>9</v>
@@ -43082,10 +43099,10 @@
     </row>
     <row r="2162" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2162" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="B2162" s="3">
-        <v>1.6520143085674979E-9</v>
+        <v>1.5836494051346807E-10</v>
       </c>
       <c r="D2162" t="s">
         <v>112</v>
@@ -43100,10 +43117,10 @@
     </row>
     <row r="2163" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2163" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B2163" s="3">
-        <v>1.5836494051346807E-10</v>
+        <v>4.5524750499172942E-7</v>
       </c>
       <c r="D2163" t="s">
         <v>112</v>
@@ -43118,10 +43135,10 @@
     </row>
     <row r="2164" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2164" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B2164" s="3">
-        <v>4.5524750499172942E-7</v>
+        <v>2.6394088838964563E-11</v>
       </c>
       <c r="D2164" t="s">
         <v>112</v>
@@ -43136,10 +43153,10 @@
     </row>
     <row r="2165" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2165" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B2165" s="3">
-        <v>2.6394088838964563E-11</v>
+        <v>2.4156210432449703E-10</v>
       </c>
       <c r="D2165" t="s">
         <v>112</v>
@@ -43152,39 +43169,39 @@
       </c>
       <c r="H2165" s="2"/>
     </row>
-    <row r="2166" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2166" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2166" s="3">
-        <v>2.4156210432449703E-10</v>
-      </c>
-      <c r="D2166" t="s">
-        <v>112</v>
-      </c>
-      <c r="E2166" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2166" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2166" s="2"/>
-    </row>
-    <row r="2167" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2"/>
-    <row r="2168" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2168" s="17" t="s">
+    <row r="2166" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="2167" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2167" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B2168" s="17" t="s">
+      <c r="B2167" s="17" t="s">
         <v>128</v>
       </c>
+    </row>
+    <row r="2168" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2168" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2168" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2168" s="2"/>
+      <c r="D2168" s="2"/>
+      <c r="E2168" s="2"/>
+      <c r="F2168" s="2"/>
+      <c r="G2168" s="2"/>
+      <c r="H2168" s="2"/>
+      <c r="I2168" s="2"/>
+      <c r="J2168" s="2"/>
+      <c r="K2168" s="2"/>
+      <c r="L2168" s="2"/>
     </row>
     <row r="2169" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2169" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2169" s="2" t="s">
-        <v>18</v>
+        <v>4</v>
+      </c>
+      <c r="B2169" s="2">
+        <v>1</v>
       </c>
       <c r="C2169" s="2"/>
       <c r="D2169" s="2"/>
@@ -43199,9 +43216,9 @@
     </row>
     <row r="2170" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2170" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2170" s="2">
+        <v>5</v>
+      </c>
+      <c r="B2170" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C2170" s="2"/>
@@ -43212,15 +43229,13 @@
       <c r="H2170" s="2"/>
       <c r="I2170" s="2"/>
       <c r="J2170" s="2"/>
-      <c r="K2170" s="2"/>
-      <c r="L2170" s="2"/>
     </row>
     <row r="2171" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2171" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2171" s="2" t="s">
-        <v>1</v>
+        <v>151</v>
+      </c>
+      <c r="B2171" s="38" t="s">
+        <v>403</v>
       </c>
       <c r="C2171" s="2"/>
       <c r="D2171" s="2"/>
@@ -43311,14 +43326,14 @@
     </row>
     <row r="2176" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2176" s="2" t="str">
-        <f>B2168</f>
+        <f>B2167</f>
         <v>methanol from biomass, burned in container ship</v>
       </c>
       <c r="B2176" s="2">
         <v>1</v>
       </c>
       <c r="C2176" s="2" t="str">
-        <f>B2169</f>
+        <f>B2168</f>
         <v>RER</v>
       </c>
       <c r="D2176" s="2"/>
@@ -43330,7 +43345,7 @@
         <v>19</v>
       </c>
       <c r="G2176" s="2" t="str">
-        <f>B2171</f>
+        <f>B2170</f>
         <v>heat</v>
       </c>
       <c r="H2176" s="2"/>
@@ -43418,8 +43433,9 @@
       <c r="A2181" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B2181" s="7">
-        <v>6.8750000000000002E-6</v>
+      <c r="B2181" s="37">
+        <f>(0.0007*20)*B2177</f>
+        <v>7.7777777777777838E-4</v>
       </c>
       <c r="D2181" s="4" t="s">
         <v>14</v>
@@ -43437,7 +43453,8 @@
         <v>71</v>
       </c>
       <c r="B2182" s="7">
-        <v>1.2499999999999999E-7</v>
+        <f>0.00695*B2177*0.1</f>
+        <v>3.8611111111111143E-5</v>
       </c>
       <c r="D2182" s="4" t="s">
         <v>14</v>

</xml_diff>